<commit_message>
[Modify] Updates input data.
</commit_message>
<xml_diff>
--- a/data/a_working/control.xlsx
+++ b/data/a_working/control.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/12b7beb4033c55a8/Documents/GitHub/hein_scraping/data/a_working/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="114_{F8364C8A-C60A-4628-9957-F973043AEB01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="16284" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -2047,8 +2041,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2111,14 +2105,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -2165,7 +2151,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2197,27 +2183,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2249,24 +2217,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2442,14 +2392,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I280"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2475,7 +2425,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2498,7 +2448,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2521,7 +2471,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2544,7 +2494,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2567,7 +2517,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2590,7 +2540,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2613,7 +2563,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2636,7 +2586,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2659,7 +2609,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2682,7 +2632,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2705,7 +2655,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2728,7 +2678,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2751,7 +2701,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2774,7 +2724,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2797,7 +2747,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2820,7 +2770,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2843,7 +2793,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2866,7 +2816,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2889,7 +2839,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2912,7 +2862,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2935,7 +2885,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2958,7 +2908,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2981,7 +2931,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -3004,7 +2954,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -3027,7 +2977,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -3050,7 +3000,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -3073,7 +3023,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -3096,7 +3046,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -3119,7 +3069,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -3142,7 +3092,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -3165,7 +3115,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -3188,7 +3138,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -3211,7 +3161,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -3234,7 +3184,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -3257,7 +3207,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -3280,7 +3230,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -3303,7 +3253,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -3326,7 +3276,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -3349,7 +3299,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -3372,7 +3322,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -3395,7 +3345,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -3418,7 +3368,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -3441,7 +3391,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -3464,7 +3414,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -3487,7 +3437,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -3510,7 +3460,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -3533,7 +3483,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -3556,7 +3506,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -3579,7 +3529,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -3602,7 +3552,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -3625,7 +3575,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -3648,7 +3598,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -3671,7 +3621,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -3694,7 +3644,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -3717,7 +3667,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -3740,7 +3690,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -3763,7 +3713,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -3786,7 +3736,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -3809,7 +3759,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -3832,7 +3782,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -3855,7 +3805,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -3878,7 +3828,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -3901,7 +3851,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -3924,7 +3874,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -3947,7 +3897,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -3970,7 +3920,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -3993,7 +3943,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -4016,7 +3966,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -4039,7 +3989,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -4062,7 +4012,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -4085,7 +4035,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -4108,7 +4058,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -4131,7 +4081,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -4154,7 +4104,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -4177,7 +4127,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -4200,7 +4150,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -4223,7 +4173,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -4246,7 +4196,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -4269,7 +4219,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -4292,7 +4242,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -4315,7 +4265,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -4338,7 +4288,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -4361,7 +4311,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -4384,7 +4334,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -4407,7 +4357,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -4430,7 +4380,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -4453,7 +4403,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -4476,7 +4426,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -4499,7 +4449,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -4522,7 +4472,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -4545,7 +4495,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -4568,7 +4518,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -4591,7 +4541,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -4614,7 +4564,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -4637,7 +4587,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -4660,7 +4610,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -4683,7 +4633,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -4706,7 +4656,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -4729,7 +4679,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -4752,7 +4702,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -4775,7 +4725,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -4798,7 +4748,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -4821,7 +4771,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -4844,7 +4794,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -4867,7 +4817,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -4890,7 +4840,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -4913,7 +4863,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -4936,7 +4886,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -4959,7 +4909,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -4982,7 +4932,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -5005,7 +4955,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -5028,7 +4978,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -5051,7 +5001,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -5074,7 +5024,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -5097,7 +5047,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -5120,7 +5070,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -5143,7 +5093,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -5166,7 +5116,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -5189,7 +5139,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -5212,7 +5162,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -5235,7 +5185,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -5258,7 +5208,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -5281,7 +5231,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -5304,7 +5254,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -5327,7 +5277,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -5350,7 +5300,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -5373,7 +5323,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -5396,7 +5346,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -5419,7 +5369,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -5442,7 +5392,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -5465,7 +5415,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -5488,7 +5438,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -5511,7 +5461,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -5534,7 +5484,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -5557,7 +5507,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -5580,7 +5530,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -5603,7 +5553,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -5626,7 +5576,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -5649,7 +5599,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -5672,7 +5622,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -5695,7 +5645,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -5718,7 +5668,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -5741,7 +5691,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -5764,7 +5714,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -5787,7 +5737,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -5810,7 +5760,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -5833,7 +5783,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -5856,7 +5806,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:8">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -5879,7 +5829,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:8">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -5902,7 +5852,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:8">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -5925,7 +5875,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:8">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -5948,7 +5898,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:8">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -5971,7 +5921,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -5994,7 +5944,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -6017,7 +5967,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -6040,7 +5990,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -6063,7 +6013,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:8">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -6086,7 +6036,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -6109,7 +6059,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:8">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -6132,7 +6082,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:8">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -6155,7 +6105,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -6178,7 +6128,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -6201,7 +6151,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -6224,7 +6174,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -6247,7 +6197,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -6270,7 +6220,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -6293,7 +6243,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -6316,7 +6266,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -6339,7 +6289,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -6362,7 +6312,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -6385,7 +6335,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -6408,7 +6358,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:8">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -6431,7 +6381,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -6454,7 +6404,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:8">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -6477,7 +6427,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:8">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -6500,7 +6450,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:8">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -6523,7 +6473,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:8">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -6546,7 +6496,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:8">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -6569,7 +6519,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:8">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -6592,7 +6542,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:8">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -6615,7 +6565,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:8">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -6638,7 +6588,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:8">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -6661,7 +6611,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:8">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -6684,7 +6634,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:8">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -6707,7 +6657,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:8">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -6730,7 +6680,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:8">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -6753,7 +6703,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:8">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -6776,7 +6726,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:8">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -6799,7 +6749,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:8">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -6822,7 +6772,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:8">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -6845,7 +6795,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:8">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -6868,7 +6818,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:8">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -6891,7 +6841,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:8">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -6914,7 +6864,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:8">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -6937,7 +6887,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:8">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -6960,7 +6910,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:8">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -6983,7 +6933,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:8">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -7006,7 +6956,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:8">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -7029,7 +6979,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:8">
       <c r="A200" s="1">
         <v>198</v>
       </c>
@@ -7052,7 +7002,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:8">
       <c r="A201" s="1">
         <v>199</v>
       </c>
@@ -7075,7 +7025,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:8">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -7098,7 +7048,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:8">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -7121,7 +7071,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:8">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -7144,7 +7094,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:8">
       <c r="A205" s="1">
         <v>203</v>
       </c>
@@ -7167,7 +7117,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:8">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -7190,7 +7140,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:8">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -7213,7 +7163,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:8">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -7236,7 +7186,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:8">
       <c r="A209" s="1">
         <v>207</v>
       </c>
@@ -7259,7 +7209,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:8">
       <c r="A210" s="1">
         <v>208</v>
       </c>
@@ -7282,7 +7232,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:8">
       <c r="A211" s="1">
         <v>209</v>
       </c>
@@ -7305,7 +7255,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:8">
       <c r="A212" s="1">
         <v>210</v>
       </c>
@@ -7328,7 +7278,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:8">
       <c r="A213" s="1">
         <v>211</v>
       </c>
@@ -7351,7 +7301,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:8">
       <c r="A214" s="1">
         <v>212</v>
       </c>
@@ -7374,7 +7324,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:8">
       <c r="A215" s="1">
         <v>213</v>
       </c>
@@ -7397,7 +7347,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:8">
       <c r="A216" s="1">
         <v>214</v>
       </c>
@@ -7420,7 +7370,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:8">
       <c r="A217" s="1">
         <v>215</v>
       </c>
@@ -7443,7 +7393,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:8">
       <c r="A218" s="1">
         <v>216</v>
       </c>
@@ -7466,7 +7416,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:8">
       <c r="A219" s="1">
         <v>217</v>
       </c>
@@ -7489,7 +7439,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:8">
       <c r="A220" s="1">
         <v>218</v>
       </c>
@@ -7512,7 +7462,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:8">
       <c r="A221" s="1">
         <v>219</v>
       </c>
@@ -7535,7 +7485,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:8">
       <c r="A222" s="1">
         <v>220</v>
       </c>
@@ -7558,7 +7508,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:8">
       <c r="A223" s="1">
         <v>221</v>
       </c>
@@ -7581,7 +7531,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:8">
       <c r="A224" s="1">
         <v>222</v>
       </c>
@@ -7604,7 +7554,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:8">
       <c r="A225" s="1">
         <v>223</v>
       </c>
@@ -7627,7 +7577,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:8">
       <c r="A226" s="1">
         <v>224</v>
       </c>
@@ -7650,7 +7600,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:8">
       <c r="A227" s="1">
         <v>225</v>
       </c>
@@ -7673,7 +7623,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:8">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -7696,7 +7646,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:8">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -7719,7 +7669,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:8">
       <c r="A230" s="1">
         <v>228</v>
       </c>
@@ -7742,7 +7692,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:8">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -7765,7 +7715,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:8">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -7788,7 +7738,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:8">
       <c r="A233" s="1">
         <v>231</v>
       </c>
@@ -7811,7 +7761,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:8">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -7834,7 +7784,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:8">
       <c r="A235" s="1">
         <v>233</v>
       </c>
@@ -7857,7 +7807,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:8">
       <c r="A236" s="1">
         <v>234</v>
       </c>
@@ -7880,7 +7830,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:8">
       <c r="A237" s="1">
         <v>235</v>
       </c>
@@ -7903,7 +7853,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:8">
       <c r="A238" s="1">
         <v>236</v>
       </c>
@@ -7926,7 +7876,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:8">
       <c r="A239" s="1">
         <v>237</v>
       </c>
@@ -7949,7 +7899,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:8">
       <c r="A240" s="1">
         <v>238</v>
       </c>
@@ -7972,7 +7922,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:8">
       <c r="A241" s="1">
         <v>239</v>
       </c>
@@ -7995,7 +7945,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:8">
       <c r="A242" s="1">
         <v>240</v>
       </c>
@@ -8018,7 +7968,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:8">
       <c r="A243" s="1">
         <v>241</v>
       </c>
@@ -8041,7 +7991,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:8">
       <c r="A244" s="1">
         <v>242</v>
       </c>
@@ -8064,7 +8014,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:8">
       <c r="A245" s="1">
         <v>243</v>
       </c>
@@ -8087,7 +8037,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:8">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -8110,7 +8060,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:8">
       <c r="A247" s="1">
         <v>245</v>
       </c>
@@ -8133,7 +8083,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:8">
       <c r="A248" s="1">
         <v>246</v>
       </c>
@@ -8156,7 +8106,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:8">
       <c r="A249" s="1">
         <v>247</v>
       </c>
@@ -8179,7 +8129,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:8">
       <c r="A250" s="1">
         <v>248</v>
       </c>
@@ -8202,7 +8152,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:8">
       <c r="A251" s="1">
         <v>249</v>
       </c>
@@ -8225,7 +8175,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:8">
       <c r="A252" s="1">
         <v>250</v>
       </c>
@@ -8248,7 +8198,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:8">
       <c r="A253" s="1">
         <v>251</v>
       </c>
@@ -8271,7 +8221,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:8">
       <c r="A254" s="1">
         <v>252</v>
       </c>
@@ -8294,7 +8244,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:8">
       <c r="A255" s="1">
         <v>253</v>
       </c>
@@ -8317,7 +8267,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:8">
       <c r="A256" s="1">
         <v>254</v>
       </c>
@@ -8340,7 +8290,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:8">
       <c r="A257" s="1">
         <v>255</v>
       </c>
@@ -8363,7 +8313,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:8">
       <c r="A258" s="1">
         <v>256</v>
       </c>
@@ -8386,7 +8336,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:8">
       <c r="A259" s="1">
         <v>257</v>
       </c>
@@ -8409,7 +8359,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:8">
       <c r="A260" s="1">
         <v>258</v>
       </c>
@@ -8432,7 +8382,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:8">
       <c r="A261" s="1">
         <v>259</v>
       </c>
@@ -8455,7 +8405,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:8">
       <c r="A262" s="1">
         <v>260</v>
       </c>
@@ -8478,7 +8428,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:8">
       <c r="A263" s="1">
         <v>261</v>
       </c>
@@ -8501,7 +8451,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:8">
       <c r="A264" s="1">
         <v>262</v>
       </c>
@@ -8524,7 +8474,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:8">
       <c r="A265" s="1">
         <v>263</v>
       </c>
@@ -8547,7 +8497,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:8">
       <c r="A266" s="1">
         <v>264</v>
       </c>
@@ -8570,7 +8520,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:8">
       <c r="A267" s="1">
         <v>265</v>
       </c>
@@ -8593,7 +8543,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:8">
       <c r="A268" s="1">
         <v>266</v>
       </c>
@@ -8616,7 +8566,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:8">
       <c r="A269" s="1">
         <v>267</v>
       </c>
@@ -8639,7 +8589,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:8">
       <c r="A270" s="1">
         <v>268</v>
       </c>
@@ -8662,7 +8612,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:8">
       <c r="A271" s="1">
         <v>269</v>
       </c>
@@ -8685,7 +8635,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:8">
       <c r="A272" s="1">
         <v>270</v>
       </c>
@@ -8708,7 +8658,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:8">
       <c r="A273" s="1">
         <v>271</v>
       </c>
@@ -8731,7 +8681,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:8">
       <c r="A274" s="1">
         <v>272</v>
       </c>
@@ -8754,7 +8704,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:8">
       <c r="A275" s="1">
         <v>273</v>
       </c>
@@ -8777,7 +8727,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:8">
       <c r="A276" s="1">
         <v>274</v>
       </c>
@@ -8800,7 +8750,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:8">
       <c r="A277" s="1">
         <v>275</v>
       </c>
@@ -8823,7 +8773,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:8">
       <c r="A278" s="1">
         <v>276</v>
       </c>
@@ -8846,7 +8796,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:8">
       <c r="A279" s="1">
         <v>277</v>
       </c>
@@ -8869,7 +8819,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:8">
       <c r="A280" s="1">
         <v>278</v>
       </c>

</xml_diff>

<commit_message>
[Modify] Code update 6/27/2021
</commit_message>
<xml_diff>
--- a/data/a_working/control.xlsx
+++ b/data/a_working/control.xlsx
@@ -1,15 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/12b7beb4033c55a8/Documents/GitHub/hein_scraping/data/a_working/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_E2FE9CCD9689AACEB0170B0C63DEF875512D97F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{279A3E7A-9021-4C9D-A11A-7CE4356B912A}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$281</definedName>
+  </definedNames>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -2050,8 +2059,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2114,6 +2123,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2160,7 +2177,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2192,9 +2209,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2226,6 +2261,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2401,14 +2454,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H281"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2434,7 +2490,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2454,7 +2510,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2474,7 +2530,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2494,7 +2550,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2514,7 +2570,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2534,7 +2590,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2554,7 +2610,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -2574,7 +2630,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2594,7 +2650,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2614,7 +2670,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2634,7 +2690,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2654,7 +2710,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2674,7 +2730,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -2694,7 +2750,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -2714,7 +2770,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -2734,7 +2790,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -2754,7 +2810,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -2774,7 +2830,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -2794,7 +2850,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -2814,7 +2870,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -2834,7 +2890,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -2854,7 +2910,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -2874,7 +2930,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -2894,7 +2950,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -2914,7 +2970,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -2934,7 +2990,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -2954,7 +3010,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -2974,7 +3030,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -2994,7 +3050,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -3014,7 +3070,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -3034,7 +3090,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -3054,7 +3110,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -3074,7 +3130,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -3094,7 +3150,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -3114,7 +3170,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -3134,7 +3190,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -3154,7 +3210,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -3174,7 +3230,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -3194,7 +3250,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -3214,7 +3270,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -3234,7 +3290,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>18</v>
       </c>
@@ -3254,7 +3310,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -3274,7 +3330,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -3294,7 +3350,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>20</v>
       </c>
@@ -3314,7 +3370,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>20</v>
       </c>
@@ -3334,7 +3390,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>20</v>
       </c>
@@ -3354,7 +3410,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>21</v>
       </c>
@@ -3374,7 +3430,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>21</v>
       </c>
@@ -3394,7 +3450,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>22</v>
       </c>
@@ -3414,7 +3470,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>22</v>
       </c>
@@ -3434,7 +3490,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>22</v>
       </c>
@@ -3454,7 +3510,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>23</v>
       </c>
@@ -3474,7 +3530,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>23</v>
       </c>
@@ -3494,7 +3550,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>24</v>
       </c>
@@ -3514,7 +3570,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>24</v>
       </c>
@@ -3534,7 +3590,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>25</v>
       </c>
@@ -3554,7 +3610,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>26</v>
       </c>
@@ -3574,7 +3630,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>26</v>
       </c>
@@ -3594,7 +3650,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>26</v>
       </c>
@@ -3614,7 +3670,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>26</v>
       </c>
@@ -3634,7 +3690,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>26</v>
       </c>
@@ -3654,7 +3710,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>27</v>
       </c>
@@ -3674,7 +3730,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>28</v>
       </c>
@@ -3694,7 +3750,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>28</v>
       </c>
@@ -3714,7 +3770,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>28</v>
       </c>
@@ -3734,7 +3790,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>28</v>
       </c>
@@ -3754,7 +3810,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>28</v>
       </c>
@@ -3774,7 +3830,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>28</v>
       </c>
@@ -3794,7 +3850,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>28</v>
       </c>
@@ -3814,7 +3870,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>22</v>
       </c>
@@ -3834,7 +3890,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>22</v>
       </c>
@@ -3854,7 +3910,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>22</v>
       </c>
@@ -3874,7 +3930,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>29</v>
       </c>
@@ -3894,7 +3950,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>29</v>
       </c>
@@ -3914,7 +3970,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>29</v>
       </c>
@@ -3934,7 +3990,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>29</v>
       </c>
@@ -3954,7 +4010,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>29</v>
       </c>
@@ -3974,7 +4030,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>29</v>
       </c>
@@ -3994,7 +4050,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>30</v>
       </c>
@@ -4014,7 +4070,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>30</v>
       </c>
@@ -4034,7 +4090,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>30</v>
       </c>
@@ -4054,7 +4110,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>30</v>
       </c>
@@ -4074,7 +4130,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>30</v>
       </c>
@@ -4094,7 +4150,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>31</v>
       </c>
@@ -4114,7 +4170,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>32</v>
       </c>
@@ -4134,7 +4190,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>32</v>
       </c>
@@ -4154,7 +4210,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>33</v>
       </c>
@@ -4174,7 +4230,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>33</v>
       </c>
@@ -4194,7 +4250,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>34</v>
       </c>
@@ -4214,7 +4270,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>34</v>
       </c>
@@ -4234,7 +4290,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>34</v>
       </c>
@@ -4254,7 +4310,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>34</v>
       </c>
@@ -4274,7 +4330,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>34</v>
       </c>
@@ -4294,7 +4350,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>34</v>
       </c>
@@ -4314,7 +4370,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>34</v>
       </c>
@@ -4334,7 +4390,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>34</v>
       </c>
@@ -4354,7 +4410,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>35</v>
       </c>
@@ -4374,7 +4430,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>35</v>
       </c>
@@ -4394,7 +4450,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>35</v>
       </c>
@@ -4414,7 +4470,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>36</v>
       </c>
@@ -4434,7 +4490,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>36</v>
       </c>
@@ -4454,7 +4510,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>36</v>
       </c>
@@ -4474,7 +4530,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>36</v>
       </c>
@@ -4494,7 +4550,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>36</v>
       </c>
@@ -4514,7 +4570,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>36</v>
       </c>
@@ -4534,7 +4590,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>37</v>
       </c>
@@ -4554,7 +4610,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>37</v>
       </c>
@@ -4574,7 +4630,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>37</v>
       </c>
@@ -4594,7 +4650,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>38</v>
       </c>
@@ -4614,7 +4670,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>38</v>
       </c>
@@ -4634,7 +4690,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>38</v>
       </c>
@@ -4654,7 +4710,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>39</v>
       </c>
@@ -4674,7 +4730,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>39</v>
       </c>
@@ -4694,7 +4750,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>39</v>
       </c>
@@ -4714,7 +4770,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>40</v>
       </c>
@@ -4734,7 +4790,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>40</v>
       </c>
@@ -4754,7 +4810,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>41</v>
       </c>
@@ -4774,7 +4830,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>41</v>
       </c>
@@ -4794,7 +4850,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>41</v>
       </c>
@@ -4814,7 +4870,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>41</v>
       </c>
@@ -4834,7 +4890,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>41</v>
       </c>
@@ -4854,7 +4910,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>42</v>
       </c>
@@ -4874,7 +4930,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>42</v>
       </c>
@@ -4894,7 +4950,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>43</v>
       </c>
@@ -4914,7 +4970,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>43</v>
       </c>
@@ -4934,7 +4990,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>43</v>
       </c>
@@ -4954,7 +5010,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>43</v>
       </c>
@@ -4974,7 +5030,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>43</v>
       </c>
@@ -4994,7 +5050,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>43</v>
       </c>
@@ -5014,7 +5070,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>44</v>
       </c>
@@ -5034,7 +5090,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>44</v>
       </c>
@@ -5054,7 +5110,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>44</v>
       </c>
@@ -5074,7 +5130,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>45</v>
       </c>
@@ -5094,7 +5150,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>46</v>
       </c>
@@ -5114,7 +5170,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="136" spans="1:7">
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>47</v>
       </c>
@@ -5134,7 +5190,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>48</v>
       </c>
@@ -5154,7 +5210,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>49</v>
       </c>
@@ -5174,7 +5230,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="139" spans="1:7">
+    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>49</v>
       </c>
@@ -5194,7 +5250,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>49</v>
       </c>
@@ -5214,7 +5270,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>49</v>
       </c>
@@ -5234,7 +5290,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>49</v>
       </c>
@@ -5254,7 +5310,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="143" spans="1:7">
+    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>49</v>
       </c>
@@ -5274,7 +5330,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="144" spans="1:7">
+    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>50</v>
       </c>
@@ -5294,7 +5350,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="145" spans="1:7">
+    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>50</v>
       </c>
@@ -5314,7 +5370,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="146" spans="1:7">
+    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>50</v>
       </c>
@@ -5334,7 +5390,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="147" spans="1:7">
+    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>50</v>
       </c>
@@ -5354,7 +5410,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="148" spans="1:7">
+    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>50</v>
       </c>
@@ -5374,7 +5430,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="149" spans="1:7">
+    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>50</v>
       </c>
@@ -5394,7 +5450,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="150" spans="1:7">
+    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>50</v>
       </c>
@@ -5414,7 +5470,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="151" spans="1:7">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>51</v>
       </c>
@@ -5434,7 +5490,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="152" spans="1:7">
+    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>51</v>
       </c>
@@ -5454,7 +5510,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="153" spans="1:7">
+    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>52</v>
       </c>
@@ -5474,7 +5530,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="154" spans="1:7">
+    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>52</v>
       </c>
@@ -5494,7 +5550,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>52</v>
       </c>
@@ -5514,7 +5570,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="156" spans="1:7">
+    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>52</v>
       </c>
@@ -5534,7 +5590,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="157" spans="1:7">
+    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>52</v>
       </c>
@@ -5554,7 +5610,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="158" spans="1:7">
+    <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>53</v>
       </c>
@@ -5574,7 +5630,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="159" spans="1:7">
+    <row r="159" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>54</v>
       </c>
@@ -5594,7 +5650,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="160" spans="1:7">
+    <row r="160" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>54</v>
       </c>
@@ -5614,7 +5670,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="161" spans="1:7">
+    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>54</v>
       </c>
@@ -5634,7 +5690,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="162" spans="1:7">
+    <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>55</v>
       </c>
@@ -5654,7 +5710,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="163" spans="1:7">
+    <row r="163" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>56</v>
       </c>
@@ -5674,7 +5730,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="164" spans="1:7">
+    <row r="164" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>21</v>
       </c>
@@ -5694,7 +5750,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="165" spans="1:7">
+    <row r="165" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>21</v>
       </c>
@@ -5714,7 +5770,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="166" spans="1:7">
+    <row r="166" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>21</v>
       </c>
@@ -5734,7 +5790,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="167" spans="1:7">
+    <row r="167" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>21</v>
       </c>
@@ -5754,7 +5810,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="168" spans="1:7">
+    <row r="168" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>57</v>
       </c>
@@ -5774,7 +5830,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="169" spans="1:7">
+    <row r="169" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>58</v>
       </c>
@@ -5794,7 +5850,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="170" spans="1:7">
+    <row r="170" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>59</v>
       </c>
@@ -5814,7 +5870,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="171" spans="1:7">
+    <row r="171" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>59</v>
       </c>
@@ -5834,7 +5890,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="172" spans="1:7">
+    <row r="172" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>59</v>
       </c>
@@ -5854,7 +5910,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="173" spans="1:7">
+    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>59</v>
       </c>
@@ -5874,7 +5930,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="174" spans="1:7">
+    <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>59</v>
       </c>
@@ -5894,7 +5950,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="175" spans="1:7">
+    <row r="175" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>60</v>
       </c>
@@ -5914,7 +5970,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="176" spans="1:7">
+    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>61</v>
       </c>
@@ -5934,7 +5990,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="177" spans="1:7">
+    <row r="177" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>61</v>
       </c>
@@ -5954,7 +6010,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="178" spans="1:7">
+    <row r="178" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>61</v>
       </c>
@@ -5974,7 +6030,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="179" spans="1:7">
+    <row r="179" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>62</v>
       </c>
@@ -5994,7 +6050,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="180" spans="1:7">
+    <row r="180" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>63</v>
       </c>
@@ -6014,7 +6070,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="181" spans="1:7">
+    <row r="181" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>63</v>
       </c>
@@ -6034,7 +6090,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="182" spans="1:7">
+    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>64</v>
       </c>
@@ -6054,7 +6110,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="183" spans="1:7">
+    <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>64</v>
       </c>
@@ -6074,7 +6130,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="184" spans="1:7">
+    <row r="184" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>65</v>
       </c>
@@ -6094,7 +6150,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="185" spans="1:7">
+    <row r="185" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>66</v>
       </c>
@@ -6114,7 +6170,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="186" spans="1:7">
+    <row r="186" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>66</v>
       </c>
@@ -6134,7 +6190,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="187" spans="1:7">
+    <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>67</v>
       </c>
@@ -6154,7 +6210,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="188" spans="1:7">
+    <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>50</v>
       </c>
@@ -6174,7 +6230,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="189" spans="1:7">
+    <row r="189" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>68</v>
       </c>
@@ -6194,7 +6250,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="190" spans="1:7">
+    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>68</v>
       </c>
@@ -6214,7 +6270,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="191" spans="1:7">
+    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>68</v>
       </c>
@@ -6234,7 +6290,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="192" spans="1:7">
+    <row r="192" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>69</v>
       </c>
@@ -6254,7 +6310,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="193" spans="1:7">
+    <row r="193" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>69</v>
       </c>
@@ -6274,7 +6330,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="194" spans="1:7">
+    <row r="194" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>69</v>
       </c>
@@ -6294,7 +6350,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="195" spans="1:7">
+    <row r="195" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>70</v>
       </c>
@@ -6314,7 +6370,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="196" spans="1:7">
+    <row r="196" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>70</v>
       </c>
@@ -6334,7 +6390,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="197" spans="1:7">
+    <row r="197" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>70</v>
       </c>
@@ -6354,7 +6410,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="198" spans="1:7">
+    <row r="198" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>70</v>
       </c>
@@ -6374,7 +6430,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="199" spans="1:7">
+    <row r="199" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>70</v>
       </c>
@@ -6394,7 +6450,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="200" spans="1:7">
+    <row r="200" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>71</v>
       </c>
@@ -6414,7 +6470,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="201" spans="1:7">
+    <row r="201" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>71</v>
       </c>
@@ -6434,7 +6490,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="202" spans="1:7">
+    <row r="202" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>71</v>
       </c>
@@ -6454,7 +6510,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="203" spans="1:7">
+    <row r="203" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>72</v>
       </c>
@@ -6474,7 +6530,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="204" spans="1:7">
+    <row r="204" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>72</v>
       </c>
@@ -6494,7 +6550,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="205" spans="1:7">
+    <row r="205" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>73</v>
       </c>
@@ -6514,7 +6570,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="206" spans="1:7">
+    <row r="206" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>73</v>
       </c>
@@ -6534,7 +6590,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="207" spans="1:7">
+    <row r="207" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>32</v>
       </c>
@@ -6554,7 +6610,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="208" spans="1:7">
+    <row r="208" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>74</v>
       </c>
@@ -6574,7 +6630,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="209" spans="1:7">
+    <row r="209" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>75</v>
       </c>
@@ -6594,7 +6650,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="210" spans="1:7">
+    <row r="210" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>75</v>
       </c>
@@ -6614,7 +6670,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="211" spans="1:7">
+    <row r="211" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>75</v>
       </c>
@@ -6634,7 +6690,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="212" spans="1:7">
+    <row r="212" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>76</v>
       </c>
@@ -6654,7 +6710,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="213" spans="1:7">
+    <row r="213" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>77</v>
       </c>
@@ -6674,7 +6730,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="214" spans="1:7">
+    <row r="214" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>77</v>
       </c>
@@ -6694,7 +6750,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="215" spans="1:7">
+    <row r="215" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>77</v>
       </c>
@@ -6714,7 +6770,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="216" spans="1:7">
+    <row r="216" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>78</v>
       </c>
@@ -6734,7 +6790,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="217" spans="1:7">
+    <row r="217" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>78</v>
       </c>
@@ -6754,7 +6810,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="218" spans="1:7">
+    <row r="218" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>78</v>
       </c>
@@ -6774,7 +6830,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="219" spans="1:7">
+    <row r="219" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>78</v>
       </c>
@@ -6794,7 +6850,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="220" spans="1:7">
+    <row r="220" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>79</v>
       </c>
@@ -6814,7 +6870,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="221" spans="1:7">
+    <row r="221" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>79</v>
       </c>
@@ -6834,7 +6890,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="222" spans="1:7">
+    <row r="222" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>79</v>
       </c>
@@ -6854,7 +6910,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="223" spans="1:7">
+    <row r="223" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>79</v>
       </c>
@@ -6874,7 +6930,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="224" spans="1:7">
+    <row r="224" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>80</v>
       </c>
@@ -6894,7 +6950,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="225" spans="1:7">
+    <row r="225" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>81</v>
       </c>
@@ -6914,7 +6970,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="226" spans="1:7">
+    <row r="226" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>82</v>
       </c>
@@ -6934,7 +6990,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="227" spans="1:7">
+    <row r="227" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>83</v>
       </c>
@@ -6954,7 +7010,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="228" spans="1:7">
+    <row r="228" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>84</v>
       </c>
@@ -6974,7 +7030,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="229" spans="1:7">
+    <row r="229" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>85</v>
       </c>
@@ -6994,7 +7050,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="230" spans="1:7">
+    <row r="230" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>85</v>
       </c>
@@ -7014,7 +7070,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="231" spans="1:7">
+    <row r="231" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>86</v>
       </c>
@@ -7034,7 +7090,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="232" spans="1:7">
+    <row r="232" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>86</v>
       </c>
@@ -7054,7 +7110,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="233" spans="1:7">
+    <row r="233" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>86</v>
       </c>
@@ -7074,7 +7130,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="234" spans="1:7">
+    <row r="234" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>87</v>
       </c>
@@ -7094,7 +7150,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="235" spans="1:7">
+    <row r="235" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>87</v>
       </c>
@@ -7114,7 +7170,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="236" spans="1:7">
+    <row r="236" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>87</v>
       </c>
@@ -7134,7 +7190,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="237" spans="1:7">
+    <row r="237" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>87</v>
       </c>
@@ -7154,7 +7210,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="238" spans="1:7">
+    <row r="238" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>88</v>
       </c>
@@ -7174,7 +7230,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="239" spans="1:7">
+    <row r="239" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>88</v>
       </c>
@@ -7194,7 +7250,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="240" spans="1:7">
+    <row r="240" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>89</v>
       </c>
@@ -7214,7 +7270,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="241" spans="1:7">
+    <row r="241" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>89</v>
       </c>
@@ -7234,7 +7290,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="242" spans="1:7">
+    <row r="242" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>89</v>
       </c>
@@ -7254,7 +7310,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="243" spans="1:7">
+    <row r="243" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>89</v>
       </c>
@@ -7274,7 +7330,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="244" spans="1:7">
+    <row r="244" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>90</v>
       </c>
@@ -7294,7 +7350,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="245" spans="1:7">
+    <row r="245" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>90</v>
       </c>
@@ -7314,7 +7370,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="246" spans="1:7">
+    <row r="246" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>91</v>
       </c>
@@ -7334,7 +7390,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="247" spans="1:7">
+    <row r="247" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>91</v>
       </c>
@@ -7354,7 +7410,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="248" spans="1:7">
+    <row r="248" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>92</v>
       </c>
@@ -7374,7 +7430,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="249" spans="1:7">
+    <row r="249" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>93</v>
       </c>
@@ -7394,7 +7450,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="250" spans="1:7">
+    <row r="250" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>94</v>
       </c>
@@ -7414,7 +7470,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="251" spans="1:7">
+    <row r="251" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>94</v>
       </c>
@@ -7434,7 +7490,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="252" spans="1:7">
+    <row r="252" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>95</v>
       </c>
@@ -7454,7 +7510,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="253" spans="1:7">
+    <row r="253" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>95</v>
       </c>
@@ -7474,7 +7530,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="254" spans="1:7">
+    <row r="254" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>96</v>
       </c>
@@ -7494,7 +7550,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="255" spans="1:7">
+    <row r="255" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>96</v>
       </c>
@@ -7514,7 +7570,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="256" spans="1:7">
+    <row r="256" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>97</v>
       </c>
@@ -7534,7 +7590,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="257" spans="1:7">
+    <row r="257" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>98</v>
       </c>
@@ -7554,7 +7610,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="258" spans="1:7">
+    <row r="258" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>99</v>
       </c>
@@ -7574,7 +7630,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="259" spans="1:7">
+    <row r="259" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>100</v>
       </c>
@@ -7594,7 +7650,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="260" spans="1:7">
+    <row r="260" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>100</v>
       </c>
@@ -7614,7 +7670,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="261" spans="1:7">
+    <row r="261" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>101</v>
       </c>
@@ -7634,7 +7690,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="262" spans="1:7">
+    <row r="262" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>102</v>
       </c>
@@ -7654,7 +7710,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="263" spans="1:7">
+    <row r="263" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>103</v>
       </c>
@@ -7674,7 +7730,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="264" spans="1:7">
+    <row r="264" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>104</v>
       </c>
@@ -7694,7 +7750,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="265" spans="1:7">
+    <row r="265" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>105</v>
       </c>
@@ -7714,7 +7770,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="266" spans="1:7">
+    <row r="266" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>106</v>
       </c>
@@ -7734,7 +7790,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="267" spans="1:7">
+    <row r="267" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>107</v>
       </c>
@@ -7754,7 +7810,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="268" spans="1:7">
+    <row r="268" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>108</v>
       </c>
@@ -7774,7 +7830,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="269" spans="1:7">
+    <row r="269" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>109</v>
       </c>
@@ -7794,7 +7850,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="270" spans="1:7">
+    <row r="270" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>110</v>
       </c>
@@ -7814,7 +7870,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="271" spans="1:7">
+    <row r="271" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>111</v>
       </c>
@@ -7834,7 +7890,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="272" spans="1:7">
+    <row r="272" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>112</v>
       </c>
@@ -7854,7 +7910,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="273" spans="1:7">
+    <row r="273" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>112</v>
       </c>
@@ -7874,7 +7930,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="274" spans="1:7">
+    <row r="274" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>113</v>
       </c>
@@ -7894,7 +7950,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="275" spans="1:7">
+    <row r="275" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>114</v>
       </c>
@@ -7914,7 +7970,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="276" spans="1:7">
+    <row r="276" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>115</v>
       </c>
@@ -7934,7 +7990,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="277" spans="1:7">
+    <row r="277" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>116</v>
       </c>
@@ -7954,7 +8010,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="278" spans="1:7">
+    <row r="278" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>117</v>
       </c>
@@ -7974,7 +8030,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="279" spans="1:7">
+    <row r="279" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>118</v>
       </c>
@@ -7994,7 +8050,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="280" spans="1:7">
+    <row r="280" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>119</v>
       </c>
@@ -8014,7 +8070,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="281" spans="1:7">
+    <row r="281" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>120</v>
       </c>
@@ -8035,6 +8091,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H281" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="1058"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>